<commit_message>
Diario de bordo codeXP turma a
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp - Acompanhamento - Turma A.xlsx
+++ b/Cronograma/CodeXp - Acompanhamento - Turma A.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
@@ -20,8 +20,171 @@
 </workbook>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rodrigo
+Catharina
+Sidney
+Renata
+Barbara
+Carlos Augusto
+Alex</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Érica Sobral
+Francielle Thiezo
+Ana Beatriz
+Lucas A Pereira
+Rafael Gomes
+Fabrício Cardoso</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Wesley Gabriel
+Angela Bonneti
+Henrique Kene
+Camila Rocha
+Alexandra Silveira
+Fernando Tolentino</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Heitor Maçã Soares
+Francielly Lima
+Victor Costa
+Denilson Santos
+Lucas Simplicio
+Amanda Santos</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Giovanni
+Emily
+Gabrielly
+Gabriel
+Lincon
+Caterine</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Paulo Ricardo
+Ana Helena
+Vivian
+Kainan
+Lucas Silveira
+Tiago</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Carla Dias
+Luciano Bispo
+Alexia Victoria
+Ingrid Nascimento
+Douglas Xavier
+Silas Oliveita</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Estevan Marcolino
+Evelin Fernanda
+Leonardo Alonso
+Ana Carolina
+Carla Naiara
+Gabriel Moraes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="127">
   <si>
     <t xml:space="preserve">REDES</t>
   </si>
@@ -353,9 +516,6 @@
     <t xml:space="preserve">Dia</t>
   </si>
   <si>
-    <t xml:space="preserve">Projetos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grupos</t>
   </si>
   <si>
@@ -371,9 +531,6 @@
     <t xml:space="preserve">Apresentação</t>
   </si>
   <si>
-    <t xml:space="preserve">Eventos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Grupo 1</t>
   </si>
   <si>
@@ -386,6 +543,9 @@
     <t xml:space="preserve">Organizar as respostas das perguntas, criar Kambam, preencher BackLog com as informações coletadas na entrevista</t>
   </si>
   <si>
+    <t xml:space="preserve">Aulas sobre AdobeXD e criação da identidade visual, e foi clonado a Home do mercado livre e foi feita a navegação, também foi definido o nome do projeto e a definição das paleta de cores do mesmo.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grupo 2</t>
   </si>
   <si>
@@ -393,9 +553,6 @@
   </si>
   <si>
     <t xml:space="preserve">Grupo 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Produtos</t>
   </si>
   <si>
     <t xml:space="preserve">Grupo 5</t>
@@ -749,7 +906,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1142,11 +1299,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1253,13 +1414,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>254520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:rowOff>20160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1272,8 +1433,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1631160" cy="1302480"/>
+          <a:off x="0" y="13680"/>
+          <a:ext cx="1416240" cy="1301760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1308,7 +1469,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="42.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="2.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="5" style="1" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="5" style="1" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="108" style="1" width="4.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="116" min="111" style="1" width="1.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="117" style="1" width="14.43"/>
@@ -7112,32 +7273,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CU34"/>
+  <dimension ref="A1:AMJ34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="84" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="84" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="84" width="26.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="7" style="84" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="18" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="85" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="86" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="50" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="86" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="73" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="86" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="76" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="87" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="94" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="88" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="1.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="84" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="84" width="21.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="84" width="26.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="84" width="22.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="7" style="84" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="17" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="85" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="86" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="49" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="86" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="72" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="86" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="75" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="87" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="93" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="98" style="88" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7529,6 +7691,8 @@
       <c r="CP2" s="93"/>
       <c r="CQ2" s="93"/>
       <c r="CR2" s="93"/>
+      <c r="CT2" s="0"/>
+      <c r="CU2" s="88"/>
     </row>
     <row r="3" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="92"/>
@@ -7828,9 +7992,7 @@
       <c r="A4" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="94" t="s">
-        <v>111</v>
-      </c>
+      <c r="B4" s="95"/>
       <c r="C4" s="95"/>
       <c r="D4" s="95"/>
       <c r="E4" s="95"/>
@@ -7875,13 +8037,13 @@
       <c r="AR4" s="95"/>
       <c r="AS4" s="95"/>
       <c r="AT4" s="95"/>
-      <c r="AU4" s="95"/>
+      <c r="AU4" s="96" t="s">
+        <v>111</v>
+      </c>
       <c r="AV4" s="96" t="s">
-        <v>112</v>
-      </c>
-      <c r="AW4" s="96" t="s">
-        <v>112</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="AW4" s="95"/>
       <c r="AX4" s="95"/>
       <c r="AY4" s="95"/>
       <c r="AZ4" s="95"/>
@@ -7903,15 +8065,15 @@
       <c r="BP4" s="95"/>
       <c r="BQ4" s="95"/>
       <c r="BR4" s="95"/>
-      <c r="BS4" s="95"/>
-      <c r="BT4" s="96" t="s">
+      <c r="BS4" s="96" t="s">
+        <v>112</v>
+      </c>
+      <c r="BT4" s="95"/>
+      <c r="BU4" s="95"/>
+      <c r="BV4" s="96" t="s">
         <v>113</v>
       </c>
-      <c r="BU4" s="95"/>
-      <c r="BV4" s="95"/>
-      <c r="BW4" s="96" t="s">
-        <v>114</v>
-      </c>
+      <c r="BW4" s="95"/>
       <c r="BX4" s="95"/>
       <c r="BY4" s="95"/>
       <c r="BZ4" s="95"/>
@@ -7934,343 +8096,338 @@
       <c r="CQ4" s="95"/>
       <c r="CR4" s="95"/>
       <c r="CS4" s="95"/>
-      <c r="CT4" s="95"/>
-      <c r="CU4" s="96" t="s">
+      <c r="CT4" s="96" t="s">
+        <v>114</v>
+      </c>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="103" customFormat="true" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="98" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="5" s="102" customFormat="true" ht="66" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="98" t="s">
+      <c r="B5" s="0"/>
+      <c r="C5" s="99" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="99" t="s">
+      <c r="D5" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="0"/>
-      <c r="D5" s="98" t="s">
+      <c r="E5" s="100" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="98" t="s">
+      <c r="F5" s="100" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="100" t="s">
+      <c r="G5" s="101"/>
+      <c r="H5" s="101"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="101"/>
+      <c r="L5" s="101"/>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="101"/>
+      <c r="Q5" s="102"/>
+      <c r="R5" s="102"/>
+      <c r="AU5" s="96"/>
+      <c r="AV5" s="96"/>
+      <c r="BS5" s="96"/>
+      <c r="BV5" s="96"/>
+      <c r="CN5" s="97"/>
+      <c r="CT5" s="96"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="103" customFormat="true" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="98" t="s">
         <v>120</v>
       </c>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="101"/>
-      <c r="S5" s="101"/>
-      <c r="AV5" s="96"/>
-      <c r="AW5" s="96"/>
-      <c r="BT5" s="96"/>
-      <c r="BW5" s="96"/>
-      <c r="CO5" s="97"/>
-      <c r="CU5" s="96"/>
-    </row>
-    <row r="6" s="102" customFormat="true" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="98"/>
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="0"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="100"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+      <c r="I6" s="101"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
+      <c r="L6" s="101"/>
+      <c r="M6" s="101"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="101"/>
+      <c r="P6" s="101"/>
+      <c r="Q6" s="102"/>
+      <c r="R6" s="102"/>
+      <c r="AU6" s="96"/>
+      <c r="AV6" s="96"/>
+      <c r="BS6" s="96"/>
+      <c r="BV6" s="96"/>
+      <c r="CN6" s="97"/>
+      <c r="CT6" s="96"/>
+      <c r="AMJ6" s="0"/>
+    </row>
+    <row r="7" s="103" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="98" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="0"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="101"/>
-      <c r="AV6" s="96"/>
-      <c r="AW6" s="96"/>
-      <c r="BT6" s="96"/>
-      <c r="BW6" s="96"/>
-      <c r="CO6" s="97"/>
-      <c r="CU6" s="96"/>
-    </row>
-    <row r="7" s="102" customFormat="true" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="98"/>
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="0"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
+      <c r="L7" s="101"/>
+      <c r="M7" s="101"/>
+      <c r="N7" s="101"/>
+      <c r="O7" s="101"/>
+      <c r="P7" s="101"/>
+      <c r="Q7" s="102"/>
+      <c r="R7" s="102"/>
+      <c r="AU7" s="96"/>
+      <c r="AV7" s="96"/>
+      <c r="BS7" s="96"/>
+      <c r="BV7" s="96"/>
+      <c r="CN7" s="97"/>
+      <c r="CT7" s="96"/>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="98" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="0"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100"/>
-      <c r="Q7" s="100"/>
-      <c r="R7" s="101"/>
-      <c r="S7" s="101"/>
-      <c r="AV7" s="96"/>
-      <c r="AW7" s="96"/>
-      <c r="BT7" s="96"/>
-      <c r="BW7" s="96"/>
-      <c r="CO7" s="97"/>
-      <c r="CU7" s="96"/>
-    </row>
-    <row r="8" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="98"/>
-      <c r="B8" s="99" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="100"/>
       <c r="F8" s="100"/>
-      <c r="G8" s="103"/>
-      <c r="H8" s="103"/>
-      <c r="I8" s="103"/>
-      <c r="J8" s="103"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="103"/>
-      <c r="M8" s="103"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="103"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="104"/>
-      <c r="S8" s="104"/>
-      <c r="V8" s="104"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="104"/>
+      <c r="N8" s="104"/>
+      <c r="O8" s="104"/>
+      <c r="P8" s="104"/>
+      <c r="Q8" s="105"/>
+      <c r="R8" s="105"/>
+      <c r="U8" s="105"/>
+      <c r="AU8" s="96"/>
       <c r="AV8" s="96"/>
-      <c r="AW8" s="96"/>
-      <c r="BT8" s="96"/>
-      <c r="BW8" s="96"/>
-      <c r="CO8" s="97"/>
-      <c r="CU8" s="96"/>
+      <c r="BS8" s="96"/>
+      <c r="BV8" s="96"/>
+      <c r="CN8" s="97"/>
+      <c r="CT8" s="96"/>
     </row>
     <row r="9" customFormat="false" ht="63" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="98" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
+      <c r="M9" s="104"/>
+      <c r="N9" s="104"/>
+      <c r="O9" s="104"/>
+      <c r="P9" s="104"/>
+      <c r="Q9" s="105"/>
+      <c r="R9" s="105"/>
+      <c r="AU9" s="96"/>
+      <c r="AV9" s="96"/>
+      <c r="BS9" s="96"/>
+      <c r="BV9" s="96"/>
+      <c r="CN9" s="97"/>
+      <c r="CT9" s="96"/>
+    </row>
+    <row r="10" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="98" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="100"/>
+      <c r="AU10" s="96"/>
+      <c r="AV10" s="96"/>
+      <c r="BS10" s="96"/>
+      <c r="BV10" s="96"/>
+      <c r="CN10" s="97"/>
+      <c r="CT10" s="96"/>
+    </row>
+    <row r="11" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="103"/>
-      <c r="M9" s="103"/>
-      <c r="N9" s="103"/>
-      <c r="O9" s="103"/>
-      <c r="P9" s="103"/>
-      <c r="Q9" s="103"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
-      <c r="AV9" s="96"/>
-      <c r="AW9" s="96"/>
-      <c r="BT9" s="96"/>
-      <c r="BW9" s="96"/>
-      <c r="CO9" s="97"/>
-      <c r="CU9" s="96"/>
-    </row>
-    <row r="10" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="98"/>
-      <c r="B10" s="99" t="s">
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="100"/>
+      <c r="AU11" s="96"/>
+      <c r="AV11" s="96"/>
+      <c r="BS11" s="96"/>
+      <c r="BV11" s="96"/>
+      <c r="CN11" s="97"/>
+      <c r="CT11" s="96"/>
+    </row>
+    <row r="12" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="98" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="100"/>
-      <c r="AV10" s="96"/>
-      <c r="AW10" s="96"/>
-      <c r="BT10" s="96"/>
-      <c r="BW10" s="96"/>
-      <c r="CO10" s="97"/>
-      <c r="CU10" s="96"/>
-    </row>
-    <row r="11" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="98"/>
-      <c r="B11" s="99" t="s">
-        <v>127</v>
-      </c>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="100"/>
-      <c r="AV11" s="96"/>
-      <c r="AW11" s="96"/>
-      <c r="BT11" s="96"/>
-      <c r="BW11" s="96"/>
-      <c r="CO11" s="97"/>
-      <c r="CU11" s="96"/>
-    </row>
-    <row r="12" customFormat="false" ht="69.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="98"/>
-      <c r="B12" s="99" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="100"/>
       <c r="F12" s="100"/>
+      <c r="AU12" s="96"/>
       <c r="AV12" s="96"/>
-      <c r="AW12" s="96"/>
-      <c r="BT12" s="96"/>
-      <c r="BW12" s="96"/>
-      <c r="CO12" s="97"/>
-      <c r="CU12" s="96"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS12" s="96"/>
+      <c r="BV12" s="96"/>
+      <c r="CN12" s="97"/>
+      <c r="CT12" s="96"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU13" s="96"/>
       <c r="AV13" s="96"/>
-      <c r="AW13" s="96"/>
-      <c r="BT13" s="96"/>
-      <c r="BW13" s="96"/>
-      <c r="CO13" s="97"/>
-      <c r="CU13" s="96"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS13" s="96"/>
+      <c r="BV13" s="96"/>
+      <c r="CN13" s="97"/>
+      <c r="CT13" s="96"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU14" s="96"/>
       <c r="AV14" s="96"/>
-      <c r="AW14" s="96"/>
-      <c r="BT14" s="96"/>
-      <c r="BW14" s="96"/>
-      <c r="CO14" s="97"/>
-      <c r="CU14" s="96"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS14" s="96"/>
+      <c r="BV14" s="96"/>
+      <c r="CN14" s="97"/>
+      <c r="CT14" s="96"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU15" s="96"/>
       <c r="AV15" s="96"/>
-      <c r="AW15" s="96"/>
-      <c r="BT15" s="96"/>
-      <c r="BW15" s="96"/>
-      <c r="CO15" s="97"/>
-      <c r="CU15" s="96"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS15" s="96"/>
+      <c r="BV15" s="96"/>
+      <c r="CN15" s="97"/>
+      <c r="CT15" s="96"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU16" s="96"/>
       <c r="AV16" s="96"/>
-      <c r="AW16" s="96"/>
-      <c r="BT16" s="96"/>
-      <c r="BW16" s="96"/>
-      <c r="CO16" s="97"/>
-      <c r="CU16" s="96"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS16" s="96"/>
+      <c r="BV16" s="96"/>
+      <c r="CN16" s="97"/>
+      <c r="CT16" s="96"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU17" s="96"/>
       <c r="AV17" s="96"/>
-      <c r="AW17" s="96"/>
-      <c r="BT17" s="96"/>
-      <c r="BW17" s="96"/>
-      <c r="CO17" s="97"/>
-      <c r="CU17" s="96"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS17" s="96"/>
+      <c r="BV17" s="96"/>
+      <c r="CN17" s="97"/>
+      <c r="CT17" s="96"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU18" s="96"/>
       <c r="AV18" s="96"/>
-      <c r="AW18" s="96"/>
-      <c r="BT18" s="96"/>
-      <c r="BW18" s="96"/>
-      <c r="CO18" s="97"/>
-      <c r="CU18" s="96"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS18" s="96"/>
+      <c r="BV18" s="96"/>
+      <c r="CN18" s="97"/>
+      <c r="CT18" s="96"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU19" s="96"/>
       <c r="AV19" s="96"/>
-      <c r="AW19" s="96"/>
-      <c r="BT19" s="96"/>
-      <c r="BW19" s="96"/>
-      <c r="CO19" s="97"/>
-      <c r="CU19" s="96"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS19" s="96"/>
+      <c r="BV19" s="96"/>
+      <c r="CN19" s="97"/>
+      <c r="CT19" s="96"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU20" s="96"/>
       <c r="AV20" s="96"/>
-      <c r="AW20" s="96"/>
-      <c r="BT20" s="96"/>
-      <c r="BW20" s="96"/>
-      <c r="CO20" s="97"/>
-      <c r="CU20" s="96"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS20" s="96"/>
+      <c r="BV20" s="96"/>
+      <c r="CN20" s="97"/>
+      <c r="CT20" s="96"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU21" s="96"/>
       <c r="AV21" s="96"/>
-      <c r="AW21" s="96"/>
-      <c r="BT21" s="96"/>
-      <c r="BW21" s="96"/>
-      <c r="CO21" s="97"/>
-      <c r="CU21" s="96"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BS21" s="96"/>
+      <c r="BV21" s="96"/>
+      <c r="CN21" s="97"/>
+      <c r="CT21" s="96"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU22" s="96"/>
       <c r="AV22" s="96"/>
-      <c r="AW22" s="96"/>
-      <c r="BT22" s="96"/>
-      <c r="BW22" s="96"/>
-      <c r="CO22" s="97"/>
-      <c r="CU22" s="96"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV23" s="105"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV24" s="105"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV25" s="105"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV26" s="105"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV27" s="105"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV28" s="105"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV29" s="105"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV30" s="105"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV31" s="105"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV32" s="105"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV33" s="105"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AV34" s="105"/>
+      <c r="BS22" s="96"/>
+      <c r="BV22" s="96"/>
+      <c r="CN22" s="97"/>
+      <c r="CT22" s="96"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU23" s="106"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU24" s="106"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU25" s="106"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU26" s="106"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU27" s="106"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU28" s="106"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU29" s="106"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU30" s="106"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU31" s="106"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU32" s="106"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU33" s="106"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AU34" s="106"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="14">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="R2:AL2"/>
     <mergeCell ref="AM2:BI2"/>
     <mergeCell ref="BJ2:CD2"/>
     <mergeCell ref="CE2:CR2"/>
+    <mergeCell ref="AU4:AU22"/>
     <mergeCell ref="AV4:AV22"/>
-    <mergeCell ref="AW4:AW22"/>
-    <mergeCell ref="BT4:BT22"/>
-    <mergeCell ref="BW4:BW22"/>
-    <mergeCell ref="CU4:CU22"/>
-    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="BS4:BS22"/>
+    <mergeCell ref="BV4:BV22"/>
+    <mergeCell ref="CT4:CT22"/>
+    <mergeCell ref="C5:C12"/>
     <mergeCell ref="D5:D12"/>
     <mergeCell ref="E5:E12"/>
     <mergeCell ref="F5:F12"/>
-    <mergeCell ref="A9:A12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -8279,6 +8436,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reformulação diario de bordo CodeXp e daily codexp dia 20
</commit_message>
<xml_diff>
--- a/Cronograma/CodeXp - Acompanhamento - Turma A.xlsx
+++ b/Cronograma/CodeXp - Acompanhamento - Turma A.xlsx
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="129">
   <si>
     <t>REDES</t>
   </si>
@@ -564,13 +564,16 @@
   </si>
   <si>
     <t>O que é Briefing, entrega do modelo Briefing, criar produto prototipado por outra equipe, ciração do trello.</t>
+  </si>
+  <si>
+    <t>Wireframes do Guffos e wireframe do projeto dos projetos da thoughtWorks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -655,14 +658,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -933,7 +928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1143,39 +1138,23 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1184,10 +1163,20 @@
     <xf numFmtId="0" fontId="11" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1209,31 +1198,34 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2089,6 +2081,390 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 16"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12573000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 14"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12573000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12573000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 10"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12573000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 8"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12573000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 6"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12573000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 4"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12573000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12573000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2376,7 +2752,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -2716,7 +3092,7 @@
       </c>
     </row>
     <row r="2" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="108"/>
+      <c r="A2" s="106"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -3042,15 +3418,15 @@
         <v>12</v>
       </c>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="109"/>
-      <c r="DH2" s="109"/>
-      <c r="DI2" s="109"/>
-      <c r="DJ2" s="109"/>
+      <c r="DG2" s="107"/>
+      <c r="DH2" s="107"/>
+      <c r="DI2" s="107"/>
+      <c r="DJ2" s="107"/>
       <c r="DK2" s="12"/>
       <c r="DL2" s="12"/>
     </row>
     <row r="3" spans="1:116" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="108"/>
+      <c r="A3" s="106"/>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
@@ -3387,7 +3763,7 @@
       <c r="A4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="108" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -3529,7 +3905,7 @@
       <c r="A5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="110"/>
+      <c r="B5" s="108"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -3669,7 +4045,7 @@
       <c r="A6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="110"/>
+      <c r="B6" s="108"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -3809,7 +4185,7 @@
       <c r="A7" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="110"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="22"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
@@ -3947,7 +4323,7 @@
       <c r="A8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="110"/>
+      <c r="B8" s="108"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
@@ -4087,7 +4463,7 @@
       <c r="A9" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="109" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="22"/>
@@ -4229,7 +4605,7 @@
       <c r="A10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="111"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
@@ -4369,7 +4745,7 @@
       <c r="A11" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="110" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="22"/>
@@ -4499,7 +4875,7 @@
       <c r="A12" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="112"/>
+      <c r="B12" s="110"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -4637,7 +5013,7 @@
       <c r="A13" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="112"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -4777,7 +5153,7 @@
       <c r="A14" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="112"/>
+      <c r="B14" s="110"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -4913,7 +5289,7 @@
       <c r="A15" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="112"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
@@ -5049,7 +5425,7 @@
       <c r="A16" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B16" s="112"/>
+      <c r="B16" s="110"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
@@ -5185,7 +5561,7 @@
       <c r="A17" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="112"/>
+      <c r="B17" s="110"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -5321,7 +5697,7 @@
       <c r="A18" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="112"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
@@ -5461,7 +5837,7 @@
       <c r="A19" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="112"/>
+      <c r="B19" s="110"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
       <c r="E19" s="22"/>
@@ -5597,7 +5973,7 @@
       <c r="A20" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="112"/>
+      <c r="B20" s="110"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -5733,7 +6109,7 @@
       <c r="A21" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="106" t="s">
+      <c r="B21" s="104" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="22"/>
@@ -5867,7 +6243,7 @@
       <c r="A22" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="106"/>
+      <c r="B22" s="104"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -6003,7 +6379,7 @@
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="B23" s="106"/>
+      <c r="B23" s="104"/>
       <c r="C23" s="22"/>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -6135,7 +6511,7 @@
       <c r="A24" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="106"/>
+      <c r="B24" s="104"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -6269,7 +6645,7 @@
       <c r="A25" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="106"/>
+      <c r="B25" s="104"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -6413,7 +6789,7 @@
       <c r="A26" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="107" t="s">
+      <c r="B26" s="105" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="22"/>
@@ -6547,7 +6923,7 @@
       <c r="A27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="107"/>
+      <c r="B27" s="105"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -6687,7 +7063,7 @@
       <c r="A28" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="107"/>
+      <c r="B28" s="105"/>
       <c r="C28" s="22"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -6819,7 +7195,7 @@
       <c r="A29" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="107"/>
+      <c r="B29" s="105"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -6947,7 +7323,7 @@
       <c r="A30" s="74" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="107"/>
+      <c r="B30" s="105"/>
       <c r="C30" s="22"/>
       <c r="D30" s="22"/>
       <c r="E30" s="22"/>
@@ -7073,7 +7449,7 @@
       <c r="A31" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="107"/>
+      <c r="B31" s="105"/>
       <c r="C31" s="22"/>
       <c r="D31" s="22"/>
       <c r="E31" s="22"/>
@@ -8168,7 +8544,7 @@
   <dimension ref="A1:AMI34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="D5" sqref="D5:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8179,7 +8555,8 @@
     <col min="4" max="4" width="26.85546875" style="78" customWidth="1"/>
     <col min="5" max="5" width="31" style="78" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" style="78" customWidth="1"/>
-    <col min="7" max="15" width="5.7109375" style="78" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="78" customWidth="1"/>
+    <col min="8" max="15" width="5.7109375" style="78" customWidth="1"/>
     <col min="16" max="45" width="5.7109375" customWidth="1"/>
     <col min="46" max="46" width="3.7109375" style="79" customWidth="1"/>
     <col min="47" max="47" width="3.7109375" style="80" customWidth="1"/>
@@ -8195,7 +8572,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1023" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="90" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="78">
@@ -8469,124 +8846,124 @@
       <c r="CP1" s="78">
         <v>104</v>
       </c>
-      <c r="CQ1" s="104">
+      <c r="CQ1" s="98">
         <v>105</v>
       </c>
       <c r="CR1" s="78">
         <v>106</v>
       </c>
-      <c r="CS1" s="105"/>
+      <c r="CS1" s="99"/>
     </row>
     <row r="2" spans="1:1023" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="91" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="112" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117"/>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="117" t="s">
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="112" t="s">
         <v>105</v>
       </c>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="117"/>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117"/>
-      <c r="U2" s="117"/>
-      <c r="V2" s="117"/>
-      <c r="W2" s="117"/>
-      <c r="X2" s="117"/>
-      <c r="Y2" s="117"/>
-      <c r="Z2" s="117"/>
-      <c r="AA2" s="117"/>
-      <c r="AB2" s="117"/>
-      <c r="AC2" s="117"/>
-      <c r="AD2" s="117"/>
-      <c r="AE2" s="117"/>
-      <c r="AF2" s="117"/>
-      <c r="AG2" s="117"/>
-      <c r="AH2" s="117"/>
-      <c r="AI2" s="117"/>
-      <c r="AJ2" s="117"/>
-      <c r="AK2" s="117" t="s">
+      <c r="Q2" s="112"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="112"/>
+      <c r="X2" s="112"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
+      <c r="AA2" s="112"/>
+      <c r="AB2" s="112"/>
+      <c r="AC2" s="112"/>
+      <c r="AD2" s="112"/>
+      <c r="AE2" s="112"/>
+      <c r="AF2" s="112"/>
+      <c r="AG2" s="112"/>
+      <c r="AH2" s="112"/>
+      <c r="AI2" s="112"/>
+      <c r="AJ2" s="112"/>
+      <c r="AK2" s="112" t="s">
         <v>106</v>
       </c>
-      <c r="AL2" s="117"/>
-      <c r="AM2" s="117"/>
-      <c r="AN2" s="117"/>
-      <c r="AO2" s="117"/>
-      <c r="AP2" s="117"/>
-      <c r="AQ2" s="117"/>
-      <c r="AR2" s="117"/>
-      <c r="AS2" s="117"/>
-      <c r="AT2" s="117"/>
-      <c r="AU2" s="117"/>
-      <c r="AV2" s="117"/>
-      <c r="AW2" s="117"/>
-      <c r="AX2" s="117"/>
-      <c r="AY2" s="117"/>
-      <c r="AZ2" s="117"/>
-      <c r="BA2" s="117"/>
-      <c r="BB2" s="117"/>
-      <c r="BC2" s="117"/>
-      <c r="BD2" s="117"/>
-      <c r="BE2" s="117"/>
-      <c r="BF2" s="117"/>
-      <c r="BG2" s="117"/>
-      <c r="BH2" s="117" t="s">
+      <c r="AL2" s="112"/>
+      <c r="AM2" s="112"/>
+      <c r="AN2" s="112"/>
+      <c r="AO2" s="112"/>
+      <c r="AP2" s="112"/>
+      <c r="AQ2" s="112"/>
+      <c r="AR2" s="112"/>
+      <c r="AS2" s="112"/>
+      <c r="AT2" s="112"/>
+      <c r="AU2" s="112"/>
+      <c r="AV2" s="112"/>
+      <c r="AW2" s="112"/>
+      <c r="AX2" s="112"/>
+      <c r="AY2" s="112"/>
+      <c r="AZ2" s="112"/>
+      <c r="BA2" s="112"/>
+      <c r="BB2" s="112"/>
+      <c r="BC2" s="112"/>
+      <c r="BD2" s="112"/>
+      <c r="BE2" s="112"/>
+      <c r="BF2" s="112"/>
+      <c r="BG2" s="112"/>
+      <c r="BH2" s="112" t="s">
         <v>107</v>
       </c>
-      <c r="BI2" s="117"/>
-      <c r="BJ2" s="117"/>
-      <c r="BK2" s="117"/>
-      <c r="BL2" s="117"/>
-      <c r="BM2" s="117"/>
-      <c r="BN2" s="117"/>
-      <c r="BO2" s="117"/>
-      <c r="BP2" s="117"/>
-      <c r="BQ2" s="117"/>
-      <c r="BR2" s="117"/>
-      <c r="BS2" s="117"/>
-      <c r="BT2" s="117"/>
-      <c r="BU2" s="117"/>
-      <c r="BV2" s="117"/>
-      <c r="BW2" s="117"/>
-      <c r="BX2" s="117"/>
-      <c r="BY2" s="117"/>
-      <c r="BZ2" s="117"/>
-      <c r="CA2" s="117"/>
-      <c r="CB2" s="117"/>
-      <c r="CC2" s="117" t="s">
+      <c r="BI2" s="112"/>
+      <c r="BJ2" s="112"/>
+      <c r="BK2" s="112"/>
+      <c r="BL2" s="112"/>
+      <c r="BM2" s="112"/>
+      <c r="BN2" s="112"/>
+      <c r="BO2" s="112"/>
+      <c r="BP2" s="112"/>
+      <c r="BQ2" s="112"/>
+      <c r="BR2" s="112"/>
+      <c r="BS2" s="112"/>
+      <c r="BT2" s="112"/>
+      <c r="BU2" s="112"/>
+      <c r="BV2" s="112"/>
+      <c r="BW2" s="112"/>
+      <c r="BX2" s="112"/>
+      <c r="BY2" s="112"/>
+      <c r="BZ2" s="112"/>
+      <c r="CA2" s="112"/>
+      <c r="CB2" s="112"/>
+      <c r="CC2" s="112" t="s">
         <v>108</v>
       </c>
-      <c r="CD2" s="117"/>
-      <c r="CE2" s="117"/>
-      <c r="CF2" s="117"/>
-      <c r="CG2" s="117"/>
-      <c r="CH2" s="117"/>
-      <c r="CI2" s="117"/>
-      <c r="CJ2" s="117"/>
-      <c r="CK2" s="117"/>
-      <c r="CL2" s="117"/>
-      <c r="CM2" s="117"/>
-      <c r="CN2" s="117"/>
-      <c r="CO2" s="117"/>
-      <c r="CP2" s="117"/>
+      <c r="CD2" s="112"/>
+      <c r="CE2" s="112"/>
+      <c r="CF2" s="112"/>
+      <c r="CG2" s="112"/>
+      <c r="CH2" s="112"/>
+      <c r="CI2" s="112"/>
+      <c r="CJ2" s="112"/>
+      <c r="CK2" s="112"/>
+      <c r="CL2" s="112"/>
+      <c r="CM2" s="112"/>
+      <c r="CN2" s="112"/>
+      <c r="CO2" s="112"/>
+      <c r="CP2" s="112"/>
     </row>
     <row r="3" spans="1:1023" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="92" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="78">
@@ -8879,87 +9256,87 @@
       </c>
     </row>
     <row r="4" spans="1:1023" s="86" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="101"/>
-      <c r="C4" s="101"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="120"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="102"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="102"/>
-      <c r="R4" s="101"/>
-      <c r="S4" s="102"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="102"/>
-      <c r="V4" s="101"/>
-      <c r="W4" s="102"/>
-      <c r="X4" s="101"/>
-      <c r="Y4" s="102"/>
-      <c r="Z4" s="101"/>
-      <c r="AA4" s="102"/>
-      <c r="AB4" s="101"/>
-      <c r="AC4" s="102"/>
-      <c r="AD4" s="101"/>
-      <c r="AE4" s="102"/>
-      <c r="AF4" s="101"/>
-      <c r="AG4" s="102"/>
-      <c r="AH4" s="101"/>
-      <c r="AI4" s="102"/>
-      <c r="AJ4" s="101"/>
-      <c r="AK4" s="102"/>
-      <c r="AL4" s="101"/>
-      <c r="AM4" s="102"/>
-      <c r="AN4" s="101"/>
-      <c r="AO4" s="102"/>
-      <c r="AP4" s="101"/>
-      <c r="AQ4" s="102"/>
-      <c r="AR4" s="101"/>
-      <c r="AS4" s="102"/>
-      <c r="AT4" s="116" t="s">
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="96"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="96"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="95"/>
+      <c r="U4" s="96"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="96"/>
+      <c r="X4" s="95"/>
+      <c r="Y4" s="96"/>
+      <c r="Z4" s="95"/>
+      <c r="AA4" s="96"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="96"/>
+      <c r="AD4" s="95"/>
+      <c r="AE4" s="96"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="96"/>
+      <c r="AH4" s="95"/>
+      <c r="AI4" s="96"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="96"/>
+      <c r="AL4" s="95"/>
+      <c r="AM4" s="96"/>
+      <c r="AN4" s="95"/>
+      <c r="AO4" s="96"/>
+      <c r="AP4" s="95"/>
+      <c r="AQ4" s="96"/>
+      <c r="AR4" s="95"/>
+      <c r="AS4" s="96"/>
+      <c r="AT4" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="AU4" s="116" t="s">
+      <c r="AU4" s="111" t="s">
         <v>111</v>
       </c>
-      <c r="AV4" s="103"/>
-      <c r="AW4" s="103"/>
-      <c r="AX4" s="103"/>
-      <c r="AY4" s="103"/>
-      <c r="AZ4" s="103"/>
-      <c r="BA4" s="103"/>
-      <c r="BB4" s="103"/>
-      <c r="BC4" s="103"/>
-      <c r="BD4" s="103"/>
-      <c r="BE4" s="103"/>
-      <c r="BF4" s="103"/>
-      <c r="BG4" s="103"/>
-      <c r="BH4" s="103"/>
-      <c r="BI4" s="103"/>
-      <c r="BJ4" s="103"/>
-      <c r="BK4" s="103"/>
-      <c r="BL4" s="103"/>
-      <c r="BM4" s="103"/>
-      <c r="BN4" s="103"/>
-      <c r="BO4" s="103"/>
-      <c r="BP4" s="103"/>
-      <c r="BQ4" s="103"/>
-      <c r="BR4" s="116" t="s">
+      <c r="AV4" s="97"/>
+      <c r="AW4" s="97"/>
+      <c r="AX4" s="97"/>
+      <c r="AY4" s="97"/>
+      <c r="AZ4" s="97"/>
+      <c r="BA4" s="97"/>
+      <c r="BB4" s="97"/>
+      <c r="BC4" s="97"/>
+      <c r="BD4" s="97"/>
+      <c r="BE4" s="97"/>
+      <c r="BF4" s="97"/>
+      <c r="BG4" s="97"/>
+      <c r="BH4" s="97"/>
+      <c r="BI4" s="97"/>
+      <c r="BJ4" s="97"/>
+      <c r="BK4" s="97"/>
+      <c r="BL4" s="97"/>
+      <c r="BM4" s="97"/>
+      <c r="BN4" s="97"/>
+      <c r="BO4" s="97"/>
+      <c r="BP4" s="97"/>
+      <c r="BQ4" s="97"/>
+      <c r="BR4" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="BS4" s="103"/>
-      <c r="BT4" s="103"/>
-      <c r="BU4" s="116" t="s">
+      <c r="BS4" s="97"/>
+      <c r="BT4" s="97"/>
+      <c r="BU4" s="111" t="s">
         <v>113</v>
       </c>
       <c r="BV4" s="85"/>
@@ -8985,327 +9362,586 @@
       <c r="CP4" s="85"/>
       <c r="CQ4" s="85"/>
       <c r="CR4" s="85"/>
-      <c r="CS4" s="116" t="s">
+      <c r="CS4" s="111" t="s">
         <v>114</v>
       </c>
       <c r="AMI4"/>
     </row>
-    <row r="5" spans="1:1023" s="90" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="99" t="s">
+    <row r="5" spans="1:1023" s="87" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="119" t="s">
+      <c r="B5" s="115" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="115" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="113" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="115" t="s">
+      <c r="E5" s="117" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="114" t="s">
+      <c r="F5" s="113" t="s">
         <v>124</v>
       </c>
-      <c r="G5" s="94"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="AT5" s="116"/>
-      <c r="AU5" s="116"/>
-      <c r="BR5" s="116"/>
-      <c r="BU5" s="116"/>
+      <c r="G5" s="113" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" s="101"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="103"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="103"/>
+      <c r="P5" s="118"/>
+      <c r="Q5" s="118"/>
+      <c r="R5" s="118"/>
+      <c r="S5" s="118"/>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="118"/>
+      <c r="W5" s="118"/>
+      <c r="X5" s="118"/>
+      <c r="Y5" s="118"/>
+      <c r="Z5" s="118"/>
+      <c r="AA5" s="118"/>
+      <c r="AB5" s="118"/>
+      <c r="AC5" s="118"/>
+      <c r="AD5" s="118"/>
+      <c r="AE5" s="118"/>
+      <c r="AF5" s="118"/>
+      <c r="AG5" s="118"/>
+      <c r="AH5" s="118"/>
+      <c r="AI5" s="118"/>
+      <c r="AJ5" s="118"/>
+      <c r="AK5" s="118"/>
+      <c r="AL5" s="118"/>
+      <c r="AM5" s="118"/>
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="118"/>
+      <c r="AS5" s="118"/>
+      <c r="AT5" s="111"/>
+      <c r="AU5" s="111"/>
+      <c r="BR5" s="111"/>
+      <c r="BU5" s="111"/>
       <c r="CM5" s="86"/>
-      <c r="CS5" s="116"/>
+      <c r="CS5" s="111"/>
       <c r="AMI5"/>
     </row>
-    <row r="6" spans="1:1023" s="90" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="99" t="s">
+    <row r="6" spans="1:1023" s="87" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="93" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="113"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="L6" s="121"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="89"/>
-      <c r="Q6" s="89"/>
-      <c r="AT6" s="116"/>
-      <c r="AU6" s="116"/>
-      <c r="BR6" s="116"/>
-      <c r="BU6" s="116"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="114"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="103"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="103"/>
+      <c r="N6" s="103"/>
+      <c r="O6" s="103"/>
+      <c r="P6" s="118"/>
+      <c r="Q6" s="118"/>
+      <c r="R6" s="118"/>
+      <c r="S6" s="118"/>
+      <c r="T6" s="118"/>
+      <c r="U6" s="118"/>
+      <c r="V6" s="118"/>
+      <c r="W6" s="118"/>
+      <c r="X6" s="118"/>
+      <c r="Y6" s="118"/>
+      <c r="Z6" s="118"/>
+      <c r="AA6" s="118"/>
+      <c r="AB6" s="118"/>
+      <c r="AC6" s="118"/>
+      <c r="AD6" s="118"/>
+      <c r="AE6" s="118"/>
+      <c r="AF6" s="118"/>
+      <c r="AG6" s="118"/>
+      <c r="AH6" s="118"/>
+      <c r="AI6" s="118"/>
+      <c r="AJ6" s="118"/>
+      <c r="AK6" s="118"/>
+      <c r="AL6" s="118"/>
+      <c r="AM6" s="118"/>
+      <c r="AN6" s="118"/>
+      <c r="AO6" s="118"/>
+      <c r="AP6" s="118"/>
+      <c r="AQ6" s="118"/>
+      <c r="AR6" s="118"/>
+      <c r="AS6" s="118"/>
+      <c r="AT6" s="111"/>
+      <c r="AU6" s="111"/>
+      <c r="BR6" s="111"/>
+      <c r="BU6" s="111"/>
       <c r="CM6" s="86"/>
-      <c r="CS6" s="116"/>
+      <c r="CS6" s="111"/>
       <c r="AMI6"/>
     </row>
-    <row r="7" spans="1:1023" s="90" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="99" t="s">
+    <row r="7" spans="1:1023" s="87" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="93" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="115"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="L7" s="88"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="89"/>
-      <c r="Q7" s="89"/>
-      <c r="AT7" s="116"/>
-      <c r="AU7" s="116"/>
-      <c r="BR7" s="116"/>
-      <c r="BU7" s="116"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="114"/>
+      <c r="G7" s="117"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="103"/>
+      <c r="K7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="118"/>
+      <c r="Q7" s="118"/>
+      <c r="R7" s="118"/>
+      <c r="S7" s="118"/>
+      <c r="T7" s="118"/>
+      <c r="U7" s="118"/>
+      <c r="V7" s="118"/>
+      <c r="W7" s="118"/>
+      <c r="X7" s="118"/>
+      <c r="Y7" s="118"/>
+      <c r="Z7" s="118"/>
+      <c r="AA7" s="118"/>
+      <c r="AB7" s="118"/>
+      <c r="AC7" s="118"/>
+      <c r="AD7" s="118"/>
+      <c r="AE7" s="118"/>
+      <c r="AF7" s="118"/>
+      <c r="AG7" s="118"/>
+      <c r="AH7" s="118"/>
+      <c r="AI7" s="118"/>
+      <c r="AJ7" s="118"/>
+      <c r="AK7" s="118"/>
+      <c r="AL7" s="118"/>
+      <c r="AM7" s="118"/>
+      <c r="AN7" s="118"/>
+      <c r="AO7" s="118"/>
+      <c r="AP7" s="118"/>
+      <c r="AQ7" s="118"/>
+      <c r="AR7" s="118"/>
+      <c r="AS7" s="118"/>
+      <c r="AT7" s="111"/>
+      <c r="AU7" s="111"/>
+      <c r="BR7" s="111"/>
+      <c r="BU7" s="111"/>
       <c r="CM7" s="86"/>
-      <c r="CS7" s="116"/>
+      <c r="CS7" s="111"/>
       <c r="AMI7"/>
     </row>
     <row r="8" spans="1:1023" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="93" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="113"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="115"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="J8" s="91"/>
-      <c r="K8" s="91"/>
-      <c r="L8" s="91"/>
-      <c r="M8" s="91"/>
-      <c r="N8" s="91"/>
-      <c r="O8" s="91"/>
-      <c r="P8" s="92"/>
-      <c r="Q8" s="92"/>
-      <c r="T8" s="92"/>
-      <c r="AT8" s="116"/>
-      <c r="AU8" s="116"/>
-      <c r="BR8" s="116"/>
-      <c r="BU8" s="116"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="117"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="119"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="120"/>
+      <c r="Q8" s="120"/>
+      <c r="R8" s="120"/>
+      <c r="S8" s="120"/>
+      <c r="T8" s="120"/>
+      <c r="U8" s="120"/>
+      <c r="V8" s="120"/>
+      <c r="W8" s="120"/>
+      <c r="X8" s="120"/>
+      <c r="Y8" s="120"/>
+      <c r="Z8" s="120"/>
+      <c r="AA8" s="120"/>
+      <c r="AB8" s="120"/>
+      <c r="AC8" s="120"/>
+      <c r="AD8" s="120"/>
+      <c r="AE8" s="120"/>
+      <c r="AF8" s="120"/>
+      <c r="AG8" s="120"/>
+      <c r="AH8" s="120"/>
+      <c r="AI8" s="120"/>
+      <c r="AJ8" s="120"/>
+      <c r="AK8" s="120"/>
+      <c r="AL8" s="120"/>
+      <c r="AM8" s="120"/>
+      <c r="AN8" s="120"/>
+      <c r="AO8" s="120"/>
+      <c r="AP8" s="120"/>
+      <c r="AQ8" s="120"/>
+      <c r="AR8" s="120"/>
+      <c r="AS8" s="120"/>
+      <c r="AT8" s="111"/>
+      <c r="AU8" s="111"/>
+      <c r="BR8" s="111"/>
+      <c r="BU8" s="111"/>
       <c r="CM8" s="86"/>
-      <c r="CS8" s="116"/>
+      <c r="CS8" s="111"/>
     </row>
     <row r="9" spans="1:1023" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="93" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="113"/>
-      <c r="D9" s="115"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="91"/>
-      <c r="I9" s="91"/>
-      <c r="J9" s="91"/>
-      <c r="K9" s="91"/>
-      <c r="L9" s="91"/>
-      <c r="M9" s="91"/>
-      <c r="N9" s="91"/>
-      <c r="O9" s="91"/>
-      <c r="P9" s="92"/>
-      <c r="Q9" s="92"/>
-      <c r="AT9" s="116"/>
-      <c r="AU9" s="116"/>
-      <c r="BR9" s="116"/>
-      <c r="BU9" s="116"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="117"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="119"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="119"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="120"/>
+      <c r="Q9" s="120"/>
+      <c r="R9" s="120"/>
+      <c r="S9" s="120"/>
+      <c r="T9" s="120"/>
+      <c r="U9" s="120"/>
+      <c r="V9" s="120"/>
+      <c r="W9" s="120"/>
+      <c r="X9" s="120"/>
+      <c r="Y9" s="120"/>
+      <c r="Z9" s="120"/>
+      <c r="AA9" s="120"/>
+      <c r="AB9" s="120"/>
+      <c r="AC9" s="120"/>
+      <c r="AD9" s="120"/>
+      <c r="AE9" s="120"/>
+      <c r="AF9" s="120"/>
+      <c r="AG9" s="120"/>
+      <c r="AH9" s="120"/>
+      <c r="AI9" s="120"/>
+      <c r="AJ9" s="120"/>
+      <c r="AK9" s="120"/>
+      <c r="AL9" s="120"/>
+      <c r="AM9" s="120"/>
+      <c r="AN9" s="120"/>
+      <c r="AO9" s="120"/>
+      <c r="AP9" s="120"/>
+      <c r="AQ9" s="120"/>
+      <c r="AR9" s="120"/>
+      <c r="AS9" s="120"/>
+      <c r="AT9" s="111"/>
+      <c r="AU9" s="111"/>
+      <c r="BR9" s="111"/>
+      <c r="BU9" s="111"/>
       <c r="CM9" s="86"/>
-      <c r="CS9" s="116"/>
+      <c r="CS9" s="111"/>
     </row>
     <row r="10" spans="1:1023" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="99" t="s">
+      <c r="A10" s="93" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="113"/>
-      <c r="C10" s="113"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="118"/>
-      <c r="AT10" s="116"/>
-      <c r="AU10" s="116"/>
-      <c r="BR10" s="116"/>
-      <c r="BU10" s="116"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="116"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="117"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="117"/>
+      <c r="H10" s="119"/>
+      <c r="I10" s="119"/>
+      <c r="J10" s="119"/>
+      <c r="K10" s="119"/>
+      <c r="L10" s="119"/>
+      <c r="M10" s="119"/>
+      <c r="N10" s="119"/>
+      <c r="O10" s="119"/>
+      <c r="P10" s="120"/>
+      <c r="Q10" s="120"/>
+      <c r="R10" s="120"/>
+      <c r="S10" s="120"/>
+      <c r="T10" s="120"/>
+      <c r="U10" s="120"/>
+      <c r="V10" s="120"/>
+      <c r="W10" s="120"/>
+      <c r="X10" s="120"/>
+      <c r="Y10" s="120"/>
+      <c r="Z10" s="120"/>
+      <c r="AA10" s="120"/>
+      <c r="AB10" s="120"/>
+      <c r="AC10" s="120"/>
+      <c r="AD10" s="120"/>
+      <c r="AE10" s="120"/>
+      <c r="AF10" s="120"/>
+      <c r="AG10" s="120"/>
+      <c r="AH10" s="120"/>
+      <c r="AI10" s="120"/>
+      <c r="AJ10" s="120"/>
+      <c r="AK10" s="120"/>
+      <c r="AL10" s="120"/>
+      <c r="AM10" s="120"/>
+      <c r="AN10" s="120"/>
+      <c r="AO10" s="120"/>
+      <c r="AP10" s="120"/>
+      <c r="AQ10" s="120"/>
+      <c r="AR10" s="120"/>
+      <c r="AS10" s="120"/>
+      <c r="AT10" s="111"/>
+      <c r="AU10" s="111"/>
+      <c r="BR10" s="111"/>
+      <c r="BU10" s="111"/>
       <c r="CM10" s="86"/>
-      <c r="CS10" s="116"/>
+      <c r="CS10" s="111"/>
     </row>
     <row r="11" spans="1:1023" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="99" t="s">
+      <c r="A11" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="113"/>
-      <c r="C11" s="113"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="118"/>
-      <c r="AT11" s="116"/>
-      <c r="AU11" s="116"/>
-      <c r="BR11" s="116"/>
-      <c r="BU11" s="116"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="119"/>
+      <c r="I11" s="119"/>
+      <c r="J11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="119"/>
+      <c r="O11" s="119"/>
+      <c r="P11" s="120"/>
+      <c r="Q11" s="120"/>
+      <c r="R11" s="120"/>
+      <c r="S11" s="120"/>
+      <c r="T11" s="120"/>
+      <c r="U11" s="120"/>
+      <c r="V11" s="120"/>
+      <c r="W11" s="120"/>
+      <c r="X11" s="120"/>
+      <c r="Y11" s="120"/>
+      <c r="Z11" s="120"/>
+      <c r="AA11" s="120"/>
+      <c r="AB11" s="120"/>
+      <c r="AC11" s="120"/>
+      <c r="AD11" s="120"/>
+      <c r="AE11" s="120"/>
+      <c r="AF11" s="120"/>
+      <c r="AG11" s="120"/>
+      <c r="AH11" s="120"/>
+      <c r="AI11" s="120"/>
+      <c r="AJ11" s="120"/>
+      <c r="AK11" s="120"/>
+      <c r="AL11" s="120"/>
+      <c r="AM11" s="120"/>
+      <c r="AN11" s="120"/>
+      <c r="AO11" s="120"/>
+      <c r="AP11" s="120"/>
+      <c r="AQ11" s="120"/>
+      <c r="AR11" s="120"/>
+      <c r="AS11" s="120"/>
+      <c r="AT11" s="111"/>
+      <c r="AU11" s="111"/>
+      <c r="BR11" s="111"/>
+      <c r="BU11" s="111"/>
       <c r="CM11" s="86"/>
-      <c r="CS11" s="116"/>
+      <c r="CS11" s="111"/>
     </row>
     <row r="12" spans="1:1023" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="115"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="118"/>
-      <c r="AT12" s="116"/>
-      <c r="AU12" s="116"/>
-      <c r="BR12" s="116"/>
-      <c r="BU12" s="116"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="119"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
+      <c r="M12" s="119"/>
+      <c r="N12" s="119"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="120"/>
+      <c r="Q12" s="120"/>
+      <c r="R12" s="120"/>
+      <c r="S12" s="120"/>
+      <c r="T12" s="120"/>
+      <c r="U12" s="120"/>
+      <c r="V12" s="120"/>
+      <c r="W12" s="120"/>
+      <c r="X12" s="120"/>
+      <c r="Y12" s="120"/>
+      <c r="Z12" s="120"/>
+      <c r="AA12" s="120"/>
+      <c r="AB12" s="120"/>
+      <c r="AC12" s="120"/>
+      <c r="AD12" s="120"/>
+      <c r="AE12" s="120"/>
+      <c r="AF12" s="120"/>
+      <c r="AG12" s="120"/>
+      <c r="AH12" s="120"/>
+      <c r="AI12" s="120"/>
+      <c r="AJ12" s="120"/>
+      <c r="AK12" s="120"/>
+      <c r="AL12" s="120"/>
+      <c r="AM12" s="120"/>
+      <c r="AN12" s="120"/>
+      <c r="AO12" s="120"/>
+      <c r="AP12" s="120"/>
+      <c r="AQ12" s="120"/>
+      <c r="AR12" s="120"/>
+      <c r="AS12" s="120"/>
+      <c r="AT12" s="111"/>
+      <c r="AU12" s="111"/>
+      <c r="BR12" s="111"/>
+      <c r="BU12" s="111"/>
       <c r="CM12" s="86"/>
-      <c r="CS12" s="116"/>
+      <c r="CS12" s="111"/>
     </row>
     <row r="13" spans="1:1023" x14ac:dyDescent="0.2">
-      <c r="A13" s="95"/>
-      <c r="AT13" s="116"/>
-      <c r="AU13" s="116"/>
-      <c r="BR13" s="116"/>
-      <c r="BU13" s="116"/>
+      <c r="A13" s="89"/>
+      <c r="AT13" s="111"/>
+      <c r="AU13" s="111"/>
+      <c r="BR13" s="111"/>
+      <c r="BU13" s="111"/>
       <c r="CM13" s="86"/>
-      <c r="CS13" s="116"/>
+      <c r="CS13" s="111"/>
     </row>
     <row r="14" spans="1:1023" x14ac:dyDescent="0.2">
-      <c r="A14" s="95"/>
-      <c r="AT14" s="116"/>
-      <c r="AU14" s="116"/>
-      <c r="BR14" s="116"/>
-      <c r="BU14" s="116"/>
+      <c r="A14" s="89"/>
+      <c r="AT14" s="111"/>
+      <c r="AU14" s="111"/>
+      <c r="BR14" s="111"/>
+      <c r="BU14" s="111"/>
       <c r="CM14" s="86"/>
-      <c r="CS14" s="116"/>
+      <c r="CS14" s="111"/>
     </row>
     <row r="15" spans="1:1023" x14ac:dyDescent="0.2">
-      <c r="AT15" s="116"/>
-      <c r="AU15" s="116"/>
-      <c r="BR15" s="116"/>
-      <c r="BU15" s="116"/>
+      <c r="AT15" s="111"/>
+      <c r="AU15" s="111"/>
+      <c r="BR15" s="111"/>
+      <c r="BU15" s="111"/>
       <c r="CM15" s="86"/>
-      <c r="CS15" s="116"/>
+      <c r="CS15" s="111"/>
     </row>
     <row r="16" spans="1:1023" x14ac:dyDescent="0.2">
-      <c r="AT16" s="116"/>
-      <c r="AU16" s="116"/>
-      <c r="BR16" s="116"/>
-      <c r="BU16" s="116"/>
+      <c r="AT16" s="111"/>
+      <c r="AU16" s="111"/>
+      <c r="BR16" s="111"/>
+      <c r="BU16" s="111"/>
       <c r="CM16" s="86"/>
-      <c r="CS16" s="116"/>
+      <c r="CS16" s="111"/>
     </row>
     <row r="17" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT17" s="116"/>
-      <c r="AU17" s="116"/>
-      <c r="BR17" s="116"/>
-      <c r="BU17" s="116"/>
+      <c r="AT17" s="111"/>
+      <c r="AU17" s="111"/>
+      <c r="BR17" s="111"/>
+      <c r="BU17" s="111"/>
       <c r="CM17" s="86"/>
-      <c r="CS17" s="116"/>
+      <c r="CS17" s="111"/>
     </row>
     <row r="18" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT18" s="116"/>
-      <c r="AU18" s="116"/>
-      <c r="BR18" s="116"/>
-      <c r="BU18" s="116"/>
+      <c r="AT18" s="111"/>
+      <c r="AU18" s="111"/>
+      <c r="BR18" s="111"/>
+      <c r="BU18" s="111"/>
       <c r="CM18" s="86"/>
-      <c r="CS18" s="116"/>
+      <c r="CS18" s="111"/>
     </row>
     <row r="19" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT19" s="116"/>
-      <c r="AU19" s="116"/>
-      <c r="BR19" s="116"/>
-      <c r="BU19" s="116"/>
+      <c r="AT19" s="111"/>
+      <c r="AU19" s="111"/>
+      <c r="BR19" s="111"/>
+      <c r="BU19" s="111"/>
       <c r="CM19" s="86"/>
-      <c r="CS19" s="116"/>
+      <c r="CS19" s="111"/>
     </row>
     <row r="20" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT20" s="116"/>
-      <c r="AU20" s="116"/>
-      <c r="BR20" s="116"/>
-      <c r="BU20" s="116"/>
+      <c r="AT20" s="111"/>
+      <c r="AU20" s="111"/>
+      <c r="BR20" s="111"/>
+      <c r="BU20" s="111"/>
       <c r="CM20" s="86"/>
-      <c r="CS20" s="116"/>
+      <c r="CS20" s="111"/>
     </row>
     <row r="21" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT21" s="116"/>
-      <c r="AU21" s="116"/>
-      <c r="BR21" s="116"/>
-      <c r="BU21" s="116"/>
+      <c r="AT21" s="111"/>
+      <c r="AU21" s="111"/>
+      <c r="BR21" s="111"/>
+      <c r="BU21" s="111"/>
       <c r="CM21" s="86"/>
-      <c r="CS21" s="116"/>
+      <c r="CS21" s="111"/>
     </row>
     <row r="22" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT22" s="116"/>
-      <c r="AU22" s="116"/>
-      <c r="BR22" s="116"/>
-      <c r="BU22" s="116"/>
+      <c r="AT22" s="111"/>
+      <c r="AU22" s="111"/>
+      <c r="BR22" s="111"/>
+      <c r="BU22" s="111"/>
       <c r="CM22" s="86"/>
-      <c r="CS22" s="116"/>
+      <c r="CS22" s="111"/>
     </row>
     <row r="23" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT23" s="93"/>
+      <c r="AT23" s="88"/>
     </row>
     <row r="24" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT24" s="93"/>
+      <c r="AT24" s="88"/>
     </row>
     <row r="25" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT25" s="93"/>
+      <c r="AT25" s="88"/>
     </row>
     <row r="26" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT26" s="93"/>
+      <c r="AT26" s="88"/>
     </row>
     <row r="27" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT27" s="93"/>
+      <c r="AT27" s="88"/>
     </row>
     <row r="28" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT28" s="93"/>
+      <c r="AT28" s="88"/>
     </row>
     <row r="29" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT29" s="93"/>
+      <c r="AT29" s="88"/>
     </row>
     <row r="30" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT30" s="93"/>
+      <c r="AT30" s="88"/>
     </row>
     <row r="31" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT31" s="93"/>
+      <c r="AT31" s="88"/>
     </row>
     <row r="32" spans="46:97" x14ac:dyDescent="0.2">
-      <c r="AT32" s="93"/>
+      <c r="AT32" s="88"/>
     </row>
     <row r="33" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT33" s="93"/>
+      <c r="AT33" s="88"/>
     </row>
     <row r="34" spans="46:46" x14ac:dyDescent="0.2">
-      <c r="AT34" s="93"/>
+      <c r="AT34" s="88"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="AU4:AU22"/>
     <mergeCell ref="BR4:BR22"/>
     <mergeCell ref="BU4:BU22"/>
@@ -9321,6 +9957,7 @@
     <mergeCell ref="D5:D12"/>
     <mergeCell ref="E5:E12"/>
     <mergeCell ref="AT4:AT22"/>
+    <mergeCell ref="G5:G12"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>